<commit_message>
Update mammal chromosome spreadsheet
</commit_message>
<xml_diff>
--- a/clades/mammalia/data/mammal_chroms_update.xlsx
+++ b/clades/mammalia/data/mammal_chroms_update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Documents/GitHub/pfsa/clades/mammalia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E837CF66-0942-A249-83B9-DB8409A9A9D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DD3199-14C5-EA4F-B5FD-C79922BC5717}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="7640" windowWidth="25580" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="460" windowWidth="25580" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mammal_chroms" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9998" uniqueCount="2487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9997" uniqueCount="2488">
   <si>
     <t>Order</t>
   </si>
@@ -7475,13 +7475,16 @@
     <t xml:space="preserve">araneus </t>
   </si>
   <si>
-    <t>Gileva 1984</t>
-  </si>
-  <si>
     <t>Wurster 1972</t>
   </si>
   <si>
     <t>Gallgher and Wommack 1992</t>
+  </si>
+  <si>
+    <t>hudsonius</t>
+  </si>
+  <si>
+    <t>Krohne 1982</t>
   </si>
 </sst>
 </file>
@@ -8354,8 +8357,8 @@
   <dimension ref="A1:Y1436"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I237" sqref="I237"/>
+      <pane ySplit="1" topLeftCell="A1006" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1033" sqref="J1033"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11506,7 +11509,7 @@
         <v>27</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="109" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -12286,7 +12289,7 @@
         <v>27</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="136" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -38193,17 +38196,20 @@
       <c r="F1031" s="2">
         <v>46</v>
       </c>
+      <c r="G1031" s="2" t="s">
+        <v>1945</v>
+      </c>
       <c r="H1031" s="2" t="s">
         <v>90</v>
       </c>
       <c r="I1031" s="2" t="s">
-        <v>724</v>
+        <v>2321</v>
       </c>
       <c r="J1031" s="2" t="s">
-        <v>27</v>
+        <v>1799</v>
       </c>
       <c r="K1031" s="2" t="s">
-        <v>2484</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="1032" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -38217,25 +38223,22 @@
         <v>723</v>
       </c>
       <c r="D1032" s="2" t="s">
-        <v>569</v>
+        <v>2486</v>
+      </c>
+      <c r="E1032" s="2">
+        <v>48</v>
       </c>
       <c r="F1032" s="2">
-        <v>45</v>
-      </c>
-      <c r="G1032" s="2" t="s">
-        <v>1945</v>
+        <v>48</v>
       </c>
       <c r="H1032" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1032" s="2" t="s">
-        <v>2321</v>
+        <v>11</v>
       </c>
       <c r="J1032" s="2" t="s">
-        <v>1799</v>
+        <v>27</v>
       </c>
       <c r="K1032" s="2" t="s">
-        <v>1930</v>
+        <v>2487</v>
       </c>
     </row>
     <row r="1033" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>